<commit_message>
Cambios en el ejercicio B
</commit_message>
<xml_diff>
--- a/Pruebas.xlsx
+++ b/Pruebas.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\OneDrive\Documentos\Octavo Semestre\Machine Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4E34A4F-ADDC-4BE1-9441-E36356746AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43308620-6017-4A42-AE25-8FBBEA5A0C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C077808F-5061-49DF-B574-4DF8094DEF52}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ejercicio A" sheetId="2" r:id="rId1"/>
+    <sheet name="Ejercicio B" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,12 +37,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>X (Años)</t>
   </si>
   <si>
     <t>Y (MDD)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Yd</t>
   </si>
 </sst>
 </file>
@@ -130,14 +137,9 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="es-MX"/>
-              <a:t>Regresión</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Ejercicio A</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="es-MX" baseline="0"/>
-              <a:t> Lineal</a:t>
-            </a:r>
-            <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -172,23 +174,453 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="5.2734898986564228E-2"/>
-          <c:y val="0.11573500333428739"/>
-          <c:w val="0.87728299446480984"/>
-          <c:h val="0.72227165942905958"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejercicio A'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Yd</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-MX"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ejercicio A'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ejercicio A'!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B4FF-4FAE-BCF3-9816B7AC2F02}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1542137087"/>
+        <c:axId val="230249855"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1542137087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="230249855"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="230249855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1542137087"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ejercicio B</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejercicio B'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Y (MDD)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -229,8 +661,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.2672910962882753E-2"/>
-                  <c:y val="-3.6302879365215382E-2"/>
+                  <c:x val="-0.16066885389326335"/>
+                  <c:y val="1.2058180227471566E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -265,7 +697,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$11</c:f>
+              <c:f>'Ejercicio B'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -304,7 +736,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$11</c:f>
+              <c:f>'Ejercicio B'!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -341,10 +773,10 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2B19-4190-A891-F9F1A9CFD673}"/>
+              <c16:uniqueId val="{00000000-9644-4B55-BD11-8AA613353976}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -356,16 +788,30 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="277484223"/>
-        <c:axId val="277485663"/>
+        <c:axId val="1540596799"/>
+        <c:axId val="1540598719"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="277484223"/>
+        <c:axId val="1540596799"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -403,12 +849,12 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277485663"/>
+        <c:crossAx val="1540598719"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="277485663"/>
+        <c:axId val="1540598719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -428,7 +874,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -465,13 +911,13 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277484223"/>
+        <c:crossAx val="1540596799"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln w="25400">
+        <a:ln>
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -479,6 +925,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -554,6 +1007,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1070,27 +1563,584 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>112465</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>78258</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>722065</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>78258</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>784860</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA3E044D-2FAF-B882-7C87-D1416A7B8BB8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EDD70C7-53CA-F1D7-3041-E401AA4762C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>373878</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>66942</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>202962</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>32759</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67B0BCCA-D1C7-5D7E-988F-7EEEADD80EE6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1427,11 +2477,115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71328969-CEFD-401F-9C5C-12B058302284}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{424530B6-A7AD-47CF-AE06-6D5A8D99E64D}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>